<commit_message>
Updated jupyter notebook to work with full version.
</commit_message>
<xml_diff>
--- a/timeHorizon.xlsx
+++ b/timeHorizon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Retirement\harp.d\HARP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DBE6E1-943B-4354-8474-064BCB81E348}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11BCFD42-74C5-4E90-9402-7EBC3DA00CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-9090" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
+    <workbookView xWindow="29520" yWindow="-6810" windowWidth="18285" windowHeight="15585" xr2:uid="{10BCA99F-290D-43B0-90F7-A2A56377E151}"/>
   </bookViews>
   <sheets>
     <sheet name="Jack" sheetId="1" r:id="rId1"/>
@@ -422,8 +422,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,9 @@
         <v>100000</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1">
+        <v>15000</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -495,7 +497,9 @@
         <v>100000</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <v>15000</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -908,8 +912,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -959,7 +963,7 @@
         <v>2023</v>
       </c>
       <c r="B2" s="1">
-        <v>20000</v>
+        <v>80000</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -974,7 +978,7 @@
         <v>2024</v>
       </c>
       <c r="B3" s="1">
-        <v>20000</v>
+        <v>80000</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -988,7 +992,9 @@
       <c r="A4">
         <v>2025</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1">
+        <v>85000</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>

</xml_diff>